<commit_message>
Added Graph results from benchmarking,updated
</commit_message>
<xml_diff>
--- a/Benchmarking Graphs/FPSvsGRIDSIZE.xlsx
+++ b/Benchmarking Graphs/FPSvsGRIDSIZE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="13395" windowHeight="7740"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="13395" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Grid Size</t>
   </si>
@@ -35,13 +35,24 @@
   <si>
     <t>5000x5000</t>
   </si>
+  <si>
+    <t>Single Threaded</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -69,8 +80,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -629,27 +641,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" customWidth="1"/>
     <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -657,7 +673,7 @@
         <v>2445</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -665,7 +681,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -673,7 +689,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -683,7 +699,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>